<commit_message>
negative numbe mod 128; 2. negative char internal reprsentation
</commit_message>
<xml_diff>
--- a/cProgramming.xlsx
+++ b/cProgramming.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Sean/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Sean/Downloads/cs240/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -87,15 +87,6 @@
 Output special character to files, like ASCII value 0, 2, is not dis</t>
   </si>
   <si>
-    <t>1. ASCII character round up and round down. 
-2. File IO</t>
-  </si>
-  <si>
-    <t>File IO: 
-FILE *fdr, *fdw;
-fopen(); fputc(); putc(); fclose()</t>
-  </si>
-  <si>
     <t>KeyLogic</t>
   </si>
   <si>
@@ -106,6 +97,21 @@
   <si>
     <t>if (ch+N) &gt; 0 :   % 128
 else if (ch+N) &lt; 0 :  ???</t>
+  </si>
+  <si>
+    <t>1. ASCII character round up and round down. 
+2. File IO
+3. char range 0-127 in C, 
+4. mod 128, negative number mod 128.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. File IO: 
+FILE *fdr, *fdw;
+fopen(); fputc(); putc(); fclose()
+2, char ch, if ch=128, %d output -128
+3.  char ch: -129  : 127 % 128 = 127
+      int ch: -129:      (-129)%128=-1
+</t>
   </si>
 </sst>
 </file>
@@ -486,7 +492,7 @@
   <dimension ref="A1:K117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -508,7 +514,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -540,19 +546,19 @@
     </row>
     <row r="2" spans="1:11" ht="114" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>13</v>

</xml_diff>